<commit_message>
1) In "BasePage.Java", JSWaiter code is added almost all of the methods.																		2) In "FilterCriteria.xlsx" file added the "TSEE" sheet and the criteria.									3) In "SA_ReviewReportCard_Test" changed the comments content.
</commit_message>
<xml_diff>
--- a/data/FilterCriteria.xlsx
+++ b/data/FilterCriteria.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wasim\git\DACAutomation\filesToUpload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wasim\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{110AE9B9-3DFA-43ED-9AF6-BFB152A3D088}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C3DE15-2059-4E32-ADB8-DD9A2AFE1036}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="6390" windowWidth="20490" xWindow="0" xr2:uid="{9FFD548A-E53B-481D-8DD6-38EDA6CC6FDB}" yWindow="1950"/>
+    <workbookView xWindow="3645" yWindow="1005" windowWidth="15915" windowHeight="6705" activeTab="1" xr2:uid="{9FFD548A-E53B-481D-8DD6-38EDA6CC6FDB}"/>
   </bookViews>
   <sheets>
-    <sheet name="SA_RRC" r:id="rId1" sheetId="1"/>
+    <sheet name="SA_RRC" sheetId="1" r:id="rId1"/>
+    <sheet name="TPSEE" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="27">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -109,20 +110,28 @@
   </si>
   <si>
     <t>Scenario7</t>
+  </si>
+  <si>
+    <t>US</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -143,16 +152,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -169,10 +180,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -207,7 +218,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -259,7 +270,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -370,21 +381,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -401,7 +412,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -453,27 +464,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567E8116-27AD-4C9D-8669-86780ACE994C}">
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567E8116-27AD-4C9D-8669-86780ACE994C}">
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="46.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="46.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -685,6 +696,90 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD2AB70-5851-4F16-A5B9-B1A62B9A70E5}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added "CA" FIlter Criteria
</commit_message>
<xml_diff>
--- a/data/FilterCriteria.xlsx
+++ b/data/FilterCriteria.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wasim\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C3DE15-2059-4E32-ADB8-DD9A2AFE1036}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331EBB94-CC7E-43B2-89C9-998501C0A17F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3645" yWindow="1005" windowWidth="15915" windowHeight="6705" activeTab="1" xr2:uid="{9FFD548A-E53B-481D-8DD6-38EDA6CC6FDB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{9FFD548A-E53B-481D-8DD6-38EDA6CC6FDB}"/>
   </bookViews>
   <sheets>
     <sheet name="SA_RRC" sheetId="1" r:id="rId1"/>
     <sheet name="TPSEE" sheetId="2" r:id="rId2"/>
+    <sheet name="CA_FIL" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="29">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -113,6 +114,12 @@
   </si>
   <si>
     <t>US</t>
+  </si>
+  <si>
+    <t>North York</t>
+  </si>
+  <si>
+    <t>State Farm - Benjamine, Victoria Park ave, M1R1R6, (416) 858-2411</t>
   </si>
 </sst>
 </file>
@@ -704,7 +711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD2AB70-5851-4F16-A5B9-B1A62B9A70E5}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -782,4 +789,111 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6967EA5-DA5A-4573-A05C-44082ECA38AA}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
CA and SA check
</commit_message>
<xml_diff>
--- a/data/FilterCriteria.xlsx
+++ b/data/FilterCriteria.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wasim\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331EBB94-CC7E-43B2-89C9-998501C0A17F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{331EBB94-CC7E-43B2-89C9-998501C0A17F}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{9FFD548A-E53B-481D-8DD6-38EDA6CC6FDB}"/>
+    <workbookView activeTab="2" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{9FFD548A-E53B-481D-8DD6-38EDA6CC6FDB}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="SA_RRC" sheetId="1" r:id="rId1"/>
-    <sheet name="TPSEE" sheetId="2" r:id="rId2"/>
-    <sheet name="CA_FIL" sheetId="3" r:id="rId3"/>
+    <sheet name="SA_RRC" r:id="rId1" sheetId="1"/>
+    <sheet name="TPSEE" r:id="rId2" sheetId="2"/>
+    <sheet name="CA_FIL" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -126,6 +126,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -159,18 +160,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -187,10 +188,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -225,7 +226,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -277,7 +278,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -388,21 +389,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -419,7 +420,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -471,15 +472,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567E8116-27AD-4C9D-8669-86780ACE994C}">
-  <dimension ref="A1:H8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567E8116-27AD-4C9D-8669-86780ACE994C}">
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -487,11 +488,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="46.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="46.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -703,13 +704,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD2AB70-5851-4F16-A5B9-B1A62B9A70E5}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD2AB70-5851-4F16-A5B9-B1A62B9A70E5}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -717,12 +718,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -786,14 +787,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6967EA5-DA5A-4573-A05C-44082ECA38AA}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6967EA5-DA5A-4573-A05C-44082ECA38AA}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -801,11 +802,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="60.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -894,6 +895,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new CA classes; Parameterized(Key driven) the testing xml with location  for Review Location competitor Set.
</commit_message>
<xml_diff>
--- a/data/FilterCriteria.xlsx
+++ b/data/FilterCriteria.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wasim\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331EBB94-CC7E-43B2-89C9-998501C0A17F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{331EBB94-CC7E-43B2-89C9-998501C0A17F}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{9FFD548A-E53B-481D-8DD6-38EDA6CC6FDB}"/>
+    <workbookView activeTab="2" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{9FFD548A-E53B-481D-8DD6-38EDA6CC6FDB}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="SA_RRC" sheetId="1" r:id="rId1"/>
-    <sheet name="TPSEE" sheetId="2" r:id="rId2"/>
-    <sheet name="CA_FIL" sheetId="3" r:id="rId3"/>
+    <sheet name="SA_RRC" r:id="rId1" sheetId="1"/>
+    <sheet name="TPSEE" r:id="rId2" sheetId="2"/>
+    <sheet name="CA_FIL" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -126,6 +126,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -159,18 +160,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -187,10 +188,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -225,7 +226,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -277,7 +278,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -388,21 +389,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -419,7 +420,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -471,15 +472,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567E8116-27AD-4C9D-8669-86780ACE994C}">
-  <dimension ref="A1:H8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567E8116-27AD-4C9D-8669-86780ACE994C}">
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -487,11 +488,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="46.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="46.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -703,13 +704,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD2AB70-5851-4F16-A5B9-B1A62B9A70E5}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD2AB70-5851-4F16-A5B9-B1A62B9A70E5}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -717,12 +718,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="5.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -786,14 +787,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6967EA5-DA5A-4573-A05C-44082ECA38AA}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6967EA5-DA5A-4573-A05C-44082ECA38AA}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -801,11 +802,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="60.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -894,6 +895,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding Social related Classes and Functions
</commit_message>
<xml_diff>
--- a/data/FilterCriteria.xlsx
+++ b/data/FilterCriteria.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wasim\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{331EBB94-CC7E-43B2-89C9-998501C0A17F}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{14680449-F875-4875-B5D1-F5217B3D236D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{9FFD548A-E53B-481D-8DD6-38EDA6CC6FDB}" yWindow="-120"/>
+    <workbookView activeTab="3" windowHeight="5640" windowWidth="20460" xWindow="30" xr2:uid="{9FFD548A-E53B-481D-8DD6-38EDA6CC6FDB}" yWindow="4830"/>
   </bookViews>
   <sheets>
     <sheet name="SA_RRC" r:id="rId1" sheetId="1"/>
     <sheet name="TPSEE" r:id="rId2" sheetId="2"/>
     <sheet name="CA_FIL" r:id="rId3" sheetId="3"/>
+    <sheet name="SA_Reports_Post" r:id="rId4" sheetId="4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="38">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -120,6 +121,33 @@
   </si>
   <si>
     <t>State Farm - Benjamine, Victoria Park ave, M1R1R6, (416) 858-2411</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Zoom</t>
+  </si>
+  <si>
+    <t>FromDate</t>
+  </si>
+  <si>
+    <t>ToDate</t>
+  </si>
+  <si>
+    <t>Day_DD</t>
+  </si>
+  <si>
+    <t>Month_MMM</t>
+  </si>
+  <si>
+    <t>Year_YYYY</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>6m</t>
   </si>
 </sst>
 </file>
@@ -162,10 +190,13 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -796,7 +827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6967EA5-DA5A-4573-A05C-44082ECA38AA}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -897,4 +928,85 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78CFF229-8D5D-4E2A-881C-A4F068EFEB39}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="9.42578125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
CA test updated and xml added
</commit_message>
<xml_diff>
--- a/data/FilterCriteria.xlsx
+++ b/data/FilterCriteria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wasim\git\DACAutomation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aneeshc\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{14680449-F875-4875-B5D1-F5217B3D236D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{F1A8C389-8DA8-41BB-9BA5-3B2F746CDA56}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="5640" windowWidth="20460" xWindow="30" xr2:uid="{9FFD548A-E53B-481D-8DD6-38EDA6CC6FDB}" yWindow="4830"/>
+    <workbookView activeTab="2" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{9FFD548A-E53B-481D-8DD6-38EDA6CC6FDB}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="SA_RRC" r:id="rId1" sheetId="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="38">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -120,9 +120,6 @@
     <t>North York</t>
   </si>
   <si>
-    <t>State Farm - Benjamine, Victoria Park ave, M1R1R6, (416) 858-2411</t>
-  </si>
-  <si>
     <t>Vendor</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>6m</t>
+  </si>
+  <si>
+    <t>Null</t>
   </si>
 </sst>
 </file>
@@ -825,10 +825,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6967EA5-DA5A-4573-A05C-44082ECA38AA}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,70 +859,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -934,7 +883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78CFF229-8D5D-4E2A-881C-A4F068EFEB39}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -951,48 +900,48 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
       <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
         <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>37</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Completed the Visiblity location calculation
</commit_message>
<xml_diff>
--- a/data/FilterCriteria.xlsx
+++ b/data/FilterCriteria.xlsx
@@ -1,40 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wasim\git\DACAutomation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abinaya\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{14680449-F875-4875-B5D1-F5217B3D236D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{E7AFD95F-0EB6-4DB1-ABD1-D52703A8CBFC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="5640" windowWidth="20460" xWindow="30" xr2:uid="{9FFD548A-E53B-481D-8DD6-38EDA6CC6FDB}" yWindow="4830"/>
+    <workbookView activeTab="3" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{9FFD548A-E53B-481D-8DD6-38EDA6CC6FDB}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="SA_RRC" r:id="rId1" sheetId="1"/>
     <sheet name="TPSEE" r:id="rId2" sheetId="2"/>
     <sheet name="CA_FIL" r:id="rId3" sheetId="3"/>
-    <sheet name="SA_Reports_Post" r:id="rId4" sheetId="4"/>
+    <sheet name="Sheet1" r:id="rId4" sheetId="5"/>
+    <sheet name="SA_Reports_Post" r:id="rId5" sheetId="4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="38">
   <si>
     <t>FilterScenarioNum</t>
   </si>
@@ -120,9 +115,6 @@
     <t>North York</t>
   </si>
   <si>
-    <t>State Farm - Benjamine, Victoria Park ave, M1R1R6, (416) 858-2411</t>
-  </si>
-  <si>
     <t>Vendor</t>
   </si>
   <si>
@@ -148,6 +140,9 @@
   </si>
   <si>
     <t>6m</t>
+  </si>
+  <si>
+    <t>State Farm - Benjamine, Victoria Park ave, M1R1R6, +14168582411</t>
   </si>
 </sst>
 </file>
@@ -825,10 +820,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6967EA5-DA5A-4573-A05C-44082ECA38AA}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,7 +835,7 @@
     <col min="5" max="5" bestFit="true" customWidth="true" width="60.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -857,73 +852,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -931,10 +880,93 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82142D6E-D5ED-405E-83AE-98222586EAD2}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78CFF229-8D5D-4E2A-881C-A4F068EFEB39}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -951,48 +983,48 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
       <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
         <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>37</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Date comparison in ROI
</commit_message>
<xml_diff>
--- a/data/FilterCriteria.xlsx
+++ b/data/FilterCriteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abinaya\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{10A94BE7-A9A3-4BAA-8DD4-38FA75C49366}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{E8405ECC-19DA-4D82-BF6A-0524222D94CD}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
     <workbookView activeTab="4" firstSheet="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{9FFD548A-E53B-481D-8DD6-38EDA6CC6FDB}" yWindow="-120"/>
   </bookViews>
@@ -143,10 +143,10 @@
     <t>Null</t>
   </si>
   <si>
-    <t>February</t>
-  </si>
-  <si>
-    <t>December</t>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
   </si>
 </sst>
 </file>
@@ -950,7 +950,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,7 +998,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="3">
         <v>2019</v>
@@ -1007,10 +1007,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F3" s="3">
-        <v>2020</v>
+        <v>2019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes for CA , TRSEE
</commit_message>
<xml_diff>
--- a/data/FilterCriteria.xlsx
+++ b/data/FilterCriteria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aneeshc\git\DACAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{AB1BB630-2BD0-4234-A0B0-70E476B1E548}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr documentId="13_ncr:1_{AECB3ADD-6E13-4EA1-B8E7-D473D1321B35}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView activeTab="3" firstSheet="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{9FFD548A-E53B-481D-8DD6-38EDA6CC6FDB}" yWindow="-120"/>
+    <workbookView activeTab="3" firstSheet="1" windowHeight="7815" windowWidth="14745" xWindow="1170" xr2:uid="{9FFD548A-E53B-481D-8DD6-38EDA6CC6FDB}" yWindow="2370"/>
   </bookViews>
   <sheets>
     <sheet name="SA_RRC" r:id="rId1" sheetId="1"/>
@@ -895,7 +895,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,7 +929,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>

</xml_diff>